<commit_message>
Scrolling, Drop Downs, Scaling
Fixed a few minor elements. Started planning website structure...
</commit_message>
<xml_diff>
--- a/src/HierachyPlanning.xlsx
+++ b/src/HierachyPlanning.xlsx
@@ -4,18 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27960" windowHeight="13110"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27960" windowHeight="13110" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Old Hierachy" sheetId="1" r:id="rId1"/>
-    <sheet name="Proposed Hierachy" sheetId="3" r:id="rId2"/>
+    <sheet name="City on a Hill" sheetId="4" r:id="rId2"/>
+    <sheet name="St. Alfreds" sheetId="5" r:id="rId3"/>
+    <sheet name="Proposed Hierachy" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="126">
   <si>
     <t>St. Pauls Old Website Herachy</t>
   </si>
@@ -255,6 +257,144 @@
   </si>
   <si>
     <t>Parking Maps are GREAT</t>
+  </si>
+  <si>
+    <t>Church</t>
+  </si>
+  <si>
+    <t>Page Hierachy</t>
+  </si>
+  <si>
+    <t>Various Notices &amp; Series Adverts</t>
+  </si>
+  <si>
+    <t>Know Jesus (About, Latest Sermon, Services)</t>
+  </si>
+  <si>
+    <t>Make Known (Connect, Serve, City News Email)</t>
+  </si>
+  <si>
+    <t>Im New</t>
+  </si>
+  <si>
+    <t>About</t>
+  </si>
+  <si>
+    <t>Vision</t>
+  </si>
+  <si>
+    <t>General Info of Startup centred around Jesus, Newcomer Event Rego &amp; Each Campus. Service Times on the Side</t>
+  </si>
+  <si>
+    <t>Want jesus Famous, Public Doctrinal Statement, 5 Flags of priorities &amp; characteristics, similar to AFT</t>
+  </si>
+  <si>
+    <t>Identity</t>
+  </si>
+  <si>
+    <t>Bible, Christ, Mission, Disciple, Culturally, Mercy, Spirit Saturated, Doctrinal Statement.</t>
+  </si>
+  <si>
+    <t>Leaders</t>
+  </si>
+  <si>
+    <t>Partners</t>
+  </si>
+  <si>
+    <t>Paid Staff, Wardens</t>
+  </si>
+  <si>
+    <t>Acts 29, Anglican Authorised from Diocese of Melbourne</t>
+  </si>
+  <si>
+    <t>Jesus</t>
+  </si>
+  <si>
+    <t>The Man, The Mission, The Message</t>
+  </si>
+  <si>
+    <t>Leads into Introducing Jesus</t>
+  </si>
+  <si>
+    <t>Baptism - 'Contact us'</t>
+  </si>
+  <si>
+    <t>Community</t>
+  </si>
+  <si>
+    <t>Gospel Communities</t>
+  </si>
+  <si>
+    <t>Organized by Neighbourhood &amp; Network, "join today"</t>
+  </si>
+  <si>
+    <t>City Kids</t>
+  </si>
+  <si>
+    <t>City Youth</t>
+  </si>
+  <si>
+    <t>No links.</t>
+  </si>
+  <si>
+    <t>Mercy</t>
+  </si>
+  <si>
+    <t>Care</t>
+  </si>
+  <si>
+    <t>Manyrooms.org.au - Outward caring for homelessness</t>
+  </si>
+  <si>
+    <t>Prayer requests!</t>
+  </si>
+  <si>
+    <t>Grow</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Serve</t>
+  </si>
+  <si>
+    <t>Leadership</t>
+  </si>
+  <si>
+    <t>Internships</t>
+  </si>
+  <si>
+    <t>Church Planting</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Sermons</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Blog</t>
+  </si>
+  <si>
+    <t>Past Sermons as well</t>
+  </si>
+  <si>
+    <t>About Worship to God, albums</t>
+  </si>
+  <si>
+    <t>Various posts about things coming up, sermon topics, news, etc</t>
+  </si>
+  <si>
+    <t>Giving, donations etc, &amp;WHY|ATTITUDE</t>
+  </si>
+  <si>
+    <t>Page Heriechy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -366,15 +506,15 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,7 +816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
@@ -698,32 +838,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="15" customHeight="1">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
     </row>
     <row r="3" spans="2:14" ht="15" customHeight="1">
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
     <row r="5" spans="2:14">
-      <c r="M5" s="10" t="s">
+      <c r="M5" s="13" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="15" customHeight="1">
-      <c r="M6" s="10"/>
+      <c r="M6" s="13"/>
     </row>
     <row r="7" spans="2:14">
       <c r="B7" s="2" t="s">
@@ -740,7 +880,7 @@
       <c r="H7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M7" s="10"/>
+      <c r="M7" s="13"/>
       <c r="N7" s="8" t="s">
         <v>43</v>
       </c>
@@ -752,13 +892,13 @@
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
     </row>
     <row r="9" spans="2:14">
       <c r="C9" s="3"/>
@@ -796,13 +936,13 @@
       <c r="F12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="H12" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
       <c r="M12" s="7" t="s">
         <v>39</v>
       </c>
@@ -849,13 +989,13 @@
       <c r="F16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="H16" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
       <c r="M16" s="7" t="s">
         <v>39</v>
       </c>
@@ -869,13 +1009,13 @@
       <c r="F17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
       <c r="M17" s="7" t="s">
         <v>39</v>
       </c>
@@ -892,13 +1032,13 @@
       <c r="F18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="12" t="s">
+      <c r="H18" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
       <c r="M18" s="7" t="s">
         <v>39</v>
       </c>
@@ -912,13 +1052,13 @@
       <c r="F19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
       <c r="M19" s="7" t="s">
         <v>39</v>
       </c>
@@ -1156,10 +1296,257 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="D7:F42"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="9" style="1"/>
+    <col min="4" max="4" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="39.75" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="4:6">
+      <c r="D7" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="4:6">
+      <c r="D9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6">
+      <c r="E10" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="4:6">
+      <c r="E11" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="4:6">
+      <c r="D13" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="4:6">
+      <c r="E14" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="4:6">
+      <c r="E15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="4:6">
+      <c r="E16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6">
+      <c r="E17" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6">
+      <c r="E18" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6">
+      <c r="D20" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6">
+      <c r="F21" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="4:6">
+      <c r="D23" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="4:6">
+      <c r="E24" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="4:6">
+      <c r="E25" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="4:6">
+      <c r="E26" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="4:6">
+      <c r="E28" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="4:6">
+      <c r="D30" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="4:6">
+      <c r="E31" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="4:6">
+      <c r="E32" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6">
+      <c r="E33" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="4:6">
+      <c r="E34" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6">
+      <c r="D36" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="4:6">
+      <c r="E38" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6">
+      <c r="E40" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="4:6">
+      <c r="D42" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C3:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:4">
+      <c r="C3" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4">
+      <c r="D4" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4">
+      <c r="C5" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:N38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1180,32 +1567,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="15" customHeight="1">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
     </row>
     <row r="3" spans="2:14" ht="15" customHeight="1">
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
     <row r="5" spans="2:14">
-      <c r="M5" s="10" t="s">
+      <c r="M5" s="13" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="15" customHeight="1">
-      <c r="M6" s="10"/>
+      <c r="M6" s="13"/>
     </row>
     <row r="7" spans="2:14">
       <c r="B7" s="2" t="s">
@@ -1222,7 +1609,7 @@
       <c r="H7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M7" s="10"/>
+      <c r="M7" s="13"/>
       <c r="N7" s="8" t="s">
         <v>43</v>
       </c>
@@ -1249,7 +1636,9 @@
     </row>
     <row r="12" spans="2:14">
       <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
+      <c r="D12" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="E12" s="4"/>
       <c r="F12" s="5"/>
     </row>

</xml_diff>